<commit_message>
Write image to excel pluss dimensions added
</commit_message>
<xml_diff>
--- a/3_Prototype.xlsx
+++ b/3_Prototype.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="195" windowWidth="18195" windowHeight="11700"/>
+    <workbookView xWindow="480" yWindow="255" windowWidth="18195" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -329,7 +329,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -356,6 +356,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF6F6BA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF3DE35D"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -373,7 +379,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -616,18 +622,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -643,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -674,6 +671,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -690,14 +688,219 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -709,7 +912,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -723,30 +926,38 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -759,203 +970,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1312,7 +1326,7 @@
   <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,7 +1344,7 @@
     <col min="12" max="12" width="6.5703125" style="1" customWidth="1"/>
     <col min="13" max="13" width="7.5703125" style="1" customWidth="1"/>
     <col min="14" max="15" width="7.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="5.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" style="1" customWidth="1"/>
     <col min="17" max="17" width="5.28515625" style="1" customWidth="1"/>
     <col min="18" max="18" width="9.140625" style="1"/>
     <col min="19" max="19" width="3.85546875" style="1" customWidth="1"/>
@@ -1342,53 +1356,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="9"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="10"/>
     </row>
     <row r="2" spans="1:23" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
     </row>
     <row r="3" spans="1:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="20"/>
-      <c r="W3" s="20"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
+      <c r="N3" s="75"/>
+      <c r="O3" s="75"/>
+      <c r="P3" s="75"/>
+      <c r="Q3" s="75"/>
+      <c r="U3" s="74"/>
+      <c r="V3" s="74"/>
+      <c r="W3" s="74"/>
     </row>
     <row r="4" spans="1:23" ht="42" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1400,38 +1414,38 @@
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="41"/>
       <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="63" t="s">
+      <c r="H4" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="64"/>
-      <c r="J4" s="65"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="69"/>
       <c r="K4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="30" t="s">
+      <c r="L4" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="44" t="s">
+      <c r="M4" s="87"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="88"/>
+      <c r="Q4" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="R4" s="45"/>
-      <c r="S4" s="46"/>
-      <c r="T4" s="22" t="s">
+      <c r="R4" s="43"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="U4" s="23"/>
+      <c r="U4" s="77"/>
       <c r="V4" s="6" t="s">
         <v>10</v>
       </c>
@@ -1439,140 +1453,137 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="75"/>
-      <c r="N5" s="75"/>
-      <c r="O5" s="75"/>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="71"/>
-      <c r="R5" s="71"/>
-      <c r="S5" s="71"/>
-      <c r="T5" s="71"/>
-      <c r="U5" s="72"/>
-      <c r="V5" s="27"/>
-      <c r="W5" s="70"/>
+    <row r="5" spans="1:23" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="35"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="71"/>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="55"/>
+      <c r="S5" s="55"/>
+      <c r="T5" s="55"/>
+      <c r="U5" s="56"/>
+      <c r="V5" s="32"/>
+      <c r="W5" s="72"/>
     </row>
-    <row r="6" spans="1:23" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="67"/>
-      <c r="R6" s="67"/>
-      <c r="S6" s="67"/>
-      <c r="T6" s="68"/>
-      <c r="U6" s="69"/>
-      <c r="V6" s="28"/>
-      <c r="W6" s="18"/>
+    <row r="6" spans="1:23" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="36"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="70"/>
+      <c r="O6" s="70"/>
+      <c r="P6" s="71"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="83"/>
+      <c r="S6" s="83"/>
+      <c r="T6" s="78"/>
+      <c r="U6" s="79"/>
+      <c r="V6" s="33"/>
+      <c r="W6" s="72"/>
     </row>
-    <row r="7" spans="1:23" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="24"/>
-      <c r="U7" s="25"/>
-      <c r="V7" s="28"/>
-      <c r="W7" s="18"/>
+    <row r="7" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="37"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="84"/>
+      <c r="R7" s="85"/>
+      <c r="S7" s="85"/>
+      <c r="T7" s="80"/>
+      <c r="U7" s="81"/>
+      <c r="V7" s="34"/>
+      <c r="W7" s="73"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="85"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="80"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="77"/>
-      <c r="Q8" s="73"/>
-      <c r="R8" s="73"/>
-      <c r="S8" s="73"/>
-      <c r="T8" s="73"/>
-      <c r="U8" s="74"/>
-      <c r="V8" s="29"/>
-      <c r="W8" s="19"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
     </row>
     <row r="13" spans="1:23" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="Q13" s="12" t="s">
+      <c r="Q13" s="13" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="V5:V8"/>
-    <mergeCell ref="W5:W8"/>
-    <mergeCell ref="L6:O8"/>
-    <mergeCell ref="G5:G8"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K5:K8"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:F8"/>
+  <mergeCells count="24">
+    <mergeCell ref="W5:W7"/>
     <mergeCell ref="U3:W3"/>
     <mergeCell ref="K2:Q2"/>
     <mergeCell ref="K3:Q3"/>
     <mergeCell ref="T4:U4"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="V5:V7"/>
     <mergeCell ref="L4:P4"/>
-    <mergeCell ref="Q6:S7"/>
-    <mergeCell ref="T6:U7"/>
-    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="D5:F7"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="M5:P6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Added save image function with dimension and resize image. Added page break
</commit_message>
<xml_diff>
--- a/3_Prototype.xlsx
+++ b/3_Prototype.xlsx
@@ -601,10 +601,14 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0"/>
+        <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -613,21 +617,19 @@
     <border>
       <left/>
       <right style="thin">
-        <color theme="0"/>
+        <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -640,7 +642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -688,10 +690,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -699,39 +697,21 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -742,10 +722,17 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -773,15 +760,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
       <protection locked="0"/>
     </xf>
@@ -830,18 +817,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -896,6 +871,14 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -967,6 +950,42 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1325,44 +1344,45 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="16.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="16" style="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="1" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="5.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="4.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="6.5703125" style="1" customWidth="1"/>
     <col min="13" max="13" width="7.5703125" style="1" customWidth="1"/>
     <col min="14" max="15" width="7.28515625" style="1" customWidth="1"/>
     <col min="16" max="16" width="6.28515625" style="1" customWidth="1"/>
     <col min="17" max="17" width="5.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="1"/>
-    <col min="19" max="19" width="3.85546875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="3" style="1" customWidth="1"/>
     <col min="20" max="20" width="9.140625" style="1"/>
-    <col min="21" max="21" width="10.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10" style="1" customWidth="1"/>
     <col min="22" max="22" width="8.42578125" style="1" customWidth="1"/>
     <col min="23" max="23" width="40.42578125" style="1" customWidth="1"/>
     <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
       <c r="K1" s="14"/>
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
@@ -1378,13 +1398,13 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="71"/>
     </row>
     <row r="3" spans="1:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="12"/>
@@ -1393,16 +1413,16 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="75"/>
-      <c r="N3" s="75"/>
-      <c r="O3" s="75"/>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="75"/>
-      <c r="U3" s="74"/>
-      <c r="V3" s="74"/>
-      <c r="W3" s="74"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="71"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="71"/>
+      <c r="U3" s="70"/>
+      <c r="V3" s="70"/>
+      <c r="W3" s="70"/>
     </row>
     <row r="4" spans="1:23" ht="42" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1414,38 +1434,38 @@
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="40"/>
-      <c r="F4" s="41"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="38"/>
       <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="67" t="s">
+      <c r="H4" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="68"/>
-      <c r="J4" s="69"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="63"/>
       <c r="K4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="86" t="s">
+      <c r="L4" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="87"/>
-      <c r="N4" s="87"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="88"/>
-      <c r="Q4" s="42" t="s">
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="83"/>
+      <c r="P4" s="84"/>
+      <c r="Q4" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="R4" s="43"/>
-      <c r="S4" s="44"/>
-      <c r="T4" s="76" t="s">
+      <c r="R4" s="40"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="U4" s="77"/>
+      <c r="U4" s="73"/>
       <c r="V4" s="6" t="s">
         <v>10</v>
       </c>
@@ -1453,80 +1473,80 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="64"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="71"/>
-      <c r="Q5" s="54"/>
-      <c r="R5" s="55"/>
-      <c r="S5" s="55"/>
-      <c r="T5" s="55"/>
-      <c r="U5" s="56"/>
-      <c r="V5" s="32"/>
-      <c r="W5" s="72"/>
+    <row r="5" spans="1:23" s="28" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="32"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="89"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="65"/>
+      <c r="Q5" s="86"/>
+      <c r="R5" s="87"/>
+      <c r="S5" s="87"/>
+      <c r="T5" s="87"/>
+      <c r="U5" s="88"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="85"/>
     </row>
     <row r="6" spans="1:23" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="70"/>
-      <c r="N6" s="70"/>
-      <c r="O6" s="70"/>
-      <c r="P6" s="71"/>
-      <c r="Q6" s="82"/>
-      <c r="R6" s="83"/>
-      <c r="S6" s="83"/>
-      <c r="T6" s="78"/>
-      <c r="U6" s="79"/>
-      <c r="V6" s="33"/>
-      <c r="W6" s="72"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="79"/>
+      <c r="S6" s="79"/>
+      <c r="T6" s="74"/>
+      <c r="U6" s="75"/>
+      <c r="V6" s="30"/>
+      <c r="W6" s="68"/>
     </row>
     <row r="7" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="84"/>
-      <c r="R7" s="85"/>
-      <c r="S7" s="85"/>
-      <c r="T7" s="80"/>
-      <c r="U7" s="81"/>
-      <c r="V7" s="34"/>
-      <c r="W7" s="73"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="90"/>
+      <c r="N7" s="91"/>
+      <c r="O7" s="92"/>
+      <c r="P7" s="93"/>
+      <c r="Q7" s="80"/>
+      <c r="R7" s="81"/>
+      <c r="S7" s="81"/>
+      <c r="T7" s="76"/>
+      <c r="U7" s="77"/>
+      <c r="V7" s="31"/>
+      <c r="W7" s="69"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>

</xml_diff>

<commit_message>
FIxed delete button not functioning right & added dimension verification via javascript
</commit_message>
<xml_diff>
--- a/3_Prototype.xlsx
+++ b/3_Prototype.xlsx
@@ -164,7 +164,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,6 +323,14 @@
       <b/>
       <sz val="24"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="161"/>
@@ -733,6 +741,72 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -745,6 +819,18 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -820,6 +906,18 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -887,105 +985,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1345,7 +1353,7 @@
   <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,11 +1384,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
       <c r="I1" s="17"/>
       <c r="J1" s="17"/>
       <c r="K1" s="14"/>
@@ -1398,13 +1406,13 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
     </row>
     <row r="3" spans="1:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="12"/>
@@ -1413,16 +1421,16 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71"/>
-      <c r="Q3" s="71"/>
-      <c r="U3" s="70"/>
-      <c r="V3" s="70"/>
-      <c r="W3" s="70"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="U3" s="34"/>
+      <c r="V3" s="34"/>
+      <c r="W3" s="34"/>
     </row>
     <row r="4" spans="1:23" ht="42" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1434,38 +1442,38 @@
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="38"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="58"/>
       <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="61" t="s">
+      <c r="H4" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="62"/>
-      <c r="J4" s="63"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="86"/>
       <c r="K4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="82" t="s">
+      <c r="L4" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="83"/>
-      <c r="P4" s="84"/>
-      <c r="Q4" s="39" t="s">
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="50"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="R4" s="40"/>
-      <c r="S4" s="41"/>
-      <c r="T4" s="72" t="s">
+      <c r="R4" s="60"/>
+      <c r="S4" s="61"/>
+      <c r="T4" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="U4" s="73"/>
+      <c r="U4" s="37"/>
       <c r="V4" s="6" t="s">
         <v>10</v>
       </c>
@@ -1474,79 +1482,79 @@
       </c>
     </row>
     <row r="5" spans="1:23" s="28" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="55"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="78"/>
       <c r="H5" s="25"/>
       <c r="I5" s="26"/>
       <c r="J5" s="27"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="89"/>
-      <c r="M5" s="64"/>
-      <c r="N5" s="64"/>
-      <c r="O5" s="64"/>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="86"/>
-      <c r="R5" s="87"/>
-      <c r="S5" s="87"/>
-      <c r="T5" s="87"/>
-      <c r="U5" s="88"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="85"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="87"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="87"/>
+      <c r="P5" s="88"/>
+      <c r="Q5" s="71"/>
+      <c r="R5" s="72"/>
+      <c r="S5" s="72"/>
+      <c r="T5" s="72"/>
+      <c r="U5" s="73"/>
+      <c r="V5" s="46"/>
+      <c r="W5" s="91"/>
     </row>
     <row r="6" spans="1:23" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="56"/>
+      <c r="A6" s="53"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="79"/>
       <c r="H6" s="21"/>
       <c r="I6" s="18"/>
       <c r="J6" s="22"/>
-      <c r="K6" s="59"/>
+      <c r="K6" s="82"/>
       <c r="L6" s="24"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
-      <c r="O6" s="66"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="78"/>
-      <c r="R6" s="79"/>
-      <c r="S6" s="79"/>
-      <c r="T6" s="74"/>
-      <c r="U6" s="75"/>
-      <c r="V6" s="30"/>
-      <c r="W6" s="68"/>
+      <c r="M6" s="89"/>
+      <c r="N6" s="89"/>
+      <c r="O6" s="89"/>
+      <c r="P6" s="90"/>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="43"/>
+      <c r="T6" s="38"/>
+      <c r="U6" s="39"/>
+      <c r="V6" s="47"/>
+      <c r="W6" s="92"/>
     </row>
     <row r="7" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="57"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="80"/>
       <c r="H7" s="19"/>
       <c r="I7" s="16"/>
       <c r="J7" s="20"/>
-      <c r="K7" s="60"/>
+      <c r="K7" s="83"/>
       <c r="L7" s="23"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="91"/>
-      <c r="O7" s="92"/>
-      <c r="P7" s="93"/>
-      <c r="Q7" s="80"/>
-      <c r="R7" s="81"/>
-      <c r="S7" s="81"/>
-      <c r="T7" s="76"/>
-      <c r="U7" s="77"/>
-      <c r="V7" s="31"/>
-      <c r="W7" s="69"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="44"/>
+      <c r="R7" s="45"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="41"/>
+      <c r="V7" s="48"/>
+      <c r="W7" s="93"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
@@ -1580,17 +1588,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="W5:W7"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="K2:Q2"/>
-    <mergeCell ref="K3:Q3"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="V5:V7"/>
-    <mergeCell ref="L4:P4"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="D1:F1"/>
@@ -1604,6 +1601,17 @@
     <mergeCell ref="K5:K7"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="M5:P6"/>
+    <mergeCell ref="W5:W7"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="K2:Q2"/>
+    <mergeCell ref="K3:Q3"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="V5:V7"/>
+    <mergeCell ref="L4:P4"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>

</xml_diff>